<commit_message>
01.guthub thay đổi nội dung
</commit_message>
<xml_diff>
--- a/01.github/Github.xlsx
+++ b/01.github/Github.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1. Tạo repository" sheetId="1" r:id="rId1"/>
     <sheet name="2. clone" sheetId="2" r:id="rId2"/>
     <sheet name="3. Câu lệnh thông dụng" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="4. config" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Repository (kho chứa) nghĩa là nơi mà bạn sẽ lưu trữ mã nguồn và một người khác có thể sao chép (clone) lại mã nguồn đó nhằm làm việc. Repository có hai loại là Local Repository (Kho chứa trên máy cá nhân) và Remote Repository (Kho chứa trên một máy chủ từ xa).</t>
   </si>
@@ -58,15 +58,6 @@
     <t>GIT GUI: chuột phải chọn Git GUI</t>
   </si>
   <si>
-    <t>add file</t>
-  </si>
-  <si>
-    <t>commit</t>
-  </si>
-  <si>
-    <t>push</t>
-  </si>
-  <si>
     <t>2. Add file</t>
   </si>
   <si>
@@ -77,13 +68,49 @@
   </si>
   <si>
     <t>git add .</t>
+  </si>
+  <si>
+    <t>3. git commit</t>
+  </si>
+  <si>
+    <t>git commit -m "nội dung message"</t>
+  </si>
+  <si>
+    <t>4. git push</t>
+  </si>
+  <si>
+    <t>Thay đổi thiết lập thông tin user</t>
+  </si>
+  <si>
+    <t>1. Set your username:</t>
+  </si>
+  <si>
+    <t>git config user.name "FIRST_NAME LAST_NAME"</t>
+  </si>
+  <si>
+    <t>Ví dụ: git config user.name "quangthaiqt"</t>
+  </si>
+  <si>
+    <t>2. Set your email address:</t>
+  </si>
+  <si>
+    <t>git config user.email "MY_NAME@example.com"</t>
+  </si>
+  <si>
+    <t>Ví dụ: git config user.email "tranquangthai188@gmail.com"</t>
+  </si>
+  <si>
+    <t>Thay đổi quyền truy cập</t>
+  </si>
+  <si>
+    <t>sau khi remove thì thực hiện push lại để thiết lập lại thông tin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +130,18 @@
       <color rgb="FF23282D"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF172B4D"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,9 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -258,6 +299,92 @@
         <a:xfrm>
           <a:off x="1295401" y="1104900"/>
           <a:ext cx="9772650" cy="3647713"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>513371</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="571500"/>
+          <a:ext cx="7828571" cy="4676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>373433</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="1924051"/>
+          <a:ext cx="4640633" cy="4324350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -580,10 +707,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K9"/>
+  <dimension ref="B2:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -603,55 +730,103 @@
     </row>
     <row r="6" spans="2:11">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:11">
       <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:11">
       <c r="C8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:11">
       <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:C4"/>
+  <dimension ref="B2:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="3:3">
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="3:3">
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3">
-      <c r="C4" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="16.5">
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>